<commit_message>
2nd day sql exercise
</commit_message>
<xml_diff>
--- a/day1/imdb.xlsx
+++ b/day1/imdb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\practiseSessions\day1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975AB778-7FE8-4E51-9A39-99BFE5CE903D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A4FCE-E8BB-4476-8B54-952F332856CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A8404972-7E91-4E77-9E30-369CB615273E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Movie</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Benn Nott</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -234,83 +240,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEFF874"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1D2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5DBF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAEF8C8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9EAFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -697,7 +646,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,37 +665,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="K1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="8"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -755,16 +704,16 @@
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>3</v>
+      <c r="G2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -776,7 +725,7 @@
       <c r="O2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="7"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -788,7 +737,7 @@
       <c r="C3">
         <v>2014</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3">
@@ -798,7 +747,7 @@
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -815,7 +764,7 @@
       <c r="O3">
         <v>3</v>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -837,7 +786,7 @@
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -854,7 +803,7 @@
       <c r="O4">
         <v>4</v>
       </c>
-      <c r="P4" s="7"/>
+      <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -876,7 +825,7 @@
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -893,7 +842,7 @@
       <c r="O5">
         <v>2</v>
       </c>
-      <c r="P5" s="7"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -915,7 +864,7 @@
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <v>4</v>
@@ -932,27 +881,27 @@
       <c r="O6">
         <v>4</v>
       </c>
-      <c r="P6" s="7"/>
+      <c r="P6" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="G8" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="G8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="L8" s="4" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="L8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -964,10 +913,10 @@
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -976,7 +925,7 @@
       <c r="H9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -1174,32 +1123,32 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="8"/>
-      <c r="L16" s="4" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="6"/>
+      <c r="L16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="4"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="7:13" x14ac:dyDescent="0.35">
       <c r="G17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="5"/>
       <c r="L17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1230,7 +1179,7 @@
       <c r="I19" t="s">
         <v>46</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="5">
         <v>2</v>
       </c>
       <c r="M19" t="s">
@@ -1277,7 +1226,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="L8:N8"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="G16:I16"/>
@@ -1286,6 +1235,7 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="M1:O1"/>
+    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:L7 E2:H2 E4:H4 E6:H6">
     <cfRule type="colorScale" priority="10">
@@ -1298,42 +1248,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:L7 E4:H4 O13 M6:O6 E6:H6">
-    <cfRule type="expression" dxfId="16" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7 P3 J3:K6">
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:E14">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:J14">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:O7">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:I22">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:N14">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C6 F3 F5">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>